<commit_message>
Latex chapter 1 and revision
</commit_message>
<xml_diff>
--- a/Docs_classes.xlsx
+++ b/Docs_classes.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865FFFDA-0B49-FF4B-8A45-5C582A541BC0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -133,7 +134,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -216,7 +217,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -291,6 +292,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -326,6 +344,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -501,68 +536,96 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="D3" sqref="D3:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.21875" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" customWidth="1"/>
+    <col min="2" max="2" width="53.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2">
         <v>2</v>
@@ -571,54 +634,54 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2">
         <v>4</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>5</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="2">
-        <v>2</v>
-      </c>
       <c r="D8" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C9" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C10" s="2">
         <v>4</v>
@@ -627,12 +690,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C11" s="2">
         <v>4</v>
@@ -641,12 +704,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C12" s="2">
         <v>4</v>
@@ -655,12 +718,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13" s="2">
         <v>4</v>
@@ -669,26 +732,26 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C15" s="2">
         <v>4</v>
@@ -697,40 +760,40 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C16" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C17" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C18" s="2">
         <v>5</v>
@@ -739,12 +802,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C19" s="2">
         <v>5</v>
@@ -753,12 +816,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C20" s="2">
         <v>5</v>
@@ -767,12 +830,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C21" s="2">
         <v>5</v>
@@ -781,40 +844,40 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C22" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C23" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C24" s="2">
         <v>6</v>
@@ -823,12 +886,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C25" s="2">
         <v>6</v>
@@ -837,12 +900,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C26" s="2">
         <v>6</v>
@@ -851,73 +914,45 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C27" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C28" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C29" s="2">
         <v>7</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
-        <v>27</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="2">
-        <v>7</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
-        <v>28</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="2">
-        <v>7</v>
-      </c>
-      <c r="D31" s="3" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adjustment towards optimizing tfidf
</commit_message>
<xml_diff>
--- a/Docs_classes.xlsx
+++ b/Docs_classes.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10917"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865FFFDA-0B49-FF4B-8A45-5C582A541BC0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE819229-5CE5-8741-8855-0C292205B61F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>admin-wp1.1_analysis_legal_institutional_environment_final</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>Tests</t>
+  </si>
+  <si>
+    <t>admin-wp2.5_matching</t>
   </si>
 </sst>
 </file>
@@ -540,7 +543,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D4"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -723,7 +726,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="C13" s="2">
         <v>4</v>

</xml_diff>